<commit_message>
Firebase (not really working, trying heroku)
</commit_message>
<xml_diff>
--- a/DictionaryApp/Mock/data/searchHistory.xlsx
+++ b/DictionaryApp/Mock/data/searchHistory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23" count="23">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
   <x:si>
     <x:t>Word</x:t>
   </x:si>
@@ -34,55 +34,22 @@
     <x:t>Antonyms</x:t>
   </x:si>
   <x:si>
-    <x:t>set</x:t>
-  </x:si>
-  <x:si>
-    <x:t>verb</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/sɛt/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"definition":"To put (something) down, to rest.","synonyms":["lay","put","set down"],"antonyms":["pick up"],"example":"Set the tray there."},{"definition":"To attach or affix (something) to something else, or in or upon a certain place.","synonyms":[],"antonyms":[],"example":"I have set my heart on running the marathon."},{"definition":"To put in a specified condition or state; to cause to be.","synonyms":[],"antonyms":[]},{"definition":"To start (a fire).","synonyms":["light"],"antonyms":["extinguish","put out","quench"]},{"definition":"To cause to stop or stick; to obstruct; to fasten to a spot.","synonyms":[],"antonyms":[],"example":"to set a coach in the mud"},{"definition":"To determine or settle.","synonyms":[],"antonyms":[],"example":"to set the rent"},{"definition":"To adjust.","synonyms":[],"antonyms":[],"example":"I set the alarm at 6 a.m."},{"definition":"To punch (a nail) into wood so that its head is below the surface.","synonyms":[],"antonyms":[]},{"definition":"To arrange with dishes and cutlery, to set the table.","synonyms":[],"antonyms":[],"example":"Please set the table for our guests."},{"definition":"To introduce or describe.","synonyms":[],"antonyms":[],"example":"I’ll tell you what happened, but first let me set the scene."},{"definition":"To locate (a play, etc.); to assign a backdrop to, geographically or temporally.","synonyms":[],"antonyms":[],"example":"He says he will set his next film in France."},{"definition":"To compile, to make (a puzzle or challenge).","synonyms":[],"antonyms":[],"example":"This crossword was set by Araucaria."},{"definition":"To prepare (a stage or film set).","synonyms":[],"antonyms":[]},{"definition":"To fit (someone) up in a situation.","synonyms":[],"antonyms":[]},{"definition":"To arrange (type).","synonyms":[],"antonyms":[],"example":"It was a complex page, but he set it quickly."},{"definition":"To devise and assign (work) to.","synonyms":[],"antonyms":[],"example":"The teacher set her students the task of drawing a foot."},{"definition":"To direct (the ball) to a teammate for an attack.","synonyms":[],"antonyms":[]},{"definition":"To solidify.","synonyms":[],"antonyms":[],"example":"The glue sets in four minutes."},{"definition":"To render stiff or solid; especially, to convert into curd; to curdle.","synonyms":[],"antonyms":[],"example":"to set milk for cheese"},{"definition":"Of a heavenly body, to disappear below the horizon of a planet, etc, as the latter rotates.","synonyms":[],"antonyms":[],"example":"The moon sets at eight o'clock tonight."},{"definition":"To defeat a contract.","synonyms":[],"antonyms":[]},{"definition":"(now followed by \"out\", as in set out) To begin to move; to go forth.","synonyms":[],"antonyms":[]},{"definition":"To produce after pollination.","synonyms":[],"antonyms":[],"example":"to set seed"},{"definition":"(of fruit) To be fixed for growth; to strike root; to begin to germinate or form.","synonyms":[],"antonyms":[]},{"definition":"(Midwestern US) To sit (be in a seated position).","synonyms":[],"antonyms":[],"example":"He sets in that chair all day."},{"definition":"To hunt game with the aid of a setter.","synonyms":[],"antonyms":[]},{"definition":"Of a dog, to indicate the position of game.","synonyms":[],"antonyms":[],"example":"The dog sets the bird."},{"definition":"To apply oneself; to undertake earnestly.","synonyms":[],"antonyms":[]},{"definition":"To fit music to words.","synonyms":[],"antonyms":[]},{"definition":"To place plants or shoots in the ground; to plant.","synonyms":[],"antonyms":[],"example":"to set pear trees in an orchard"},{"definition":"To become fixed or rigid; to be fastened.","synonyms":[],"antonyms":[]},{"definition":"To have a certain direction of motion; to flow; to move on; to tend.","synonyms":[],"antonyms":[],"example":"The current sets to the north; the tide sets to the windward."},{"definition":"(country dancing) To acknowledge a dancing partner by facing him or her and moving first to one side and then to the other, while she or he does the opposite.","synonyms":[],"antonyms":[],"example":"Set to partners! was the next instruction from the caller."},{"definition":"To place or fix in a setting.","synonyms":[],"antonyms":[],"example":"to set a precious stone in a border of metal"},{"definition":"To put in order in a particular manner; to prepare.","synonyms":[],"antonyms":[],"example":"to set (that is, to hone) a razor"},{"definition":"To extend and bring into position; to spread.","synonyms":[],"antonyms":[],"example":"to set the sails of a ship"},{"definition":"To give a pitch to, as a tune; to start by fixing the keynote.","synonyms":[],"antonyms":[],"example":"to set a psalm"},{"definition":"To reduce from a dislocated or fractured state.","synonyms":[],"antonyms":[],"example":"to set a broken bone"},{"definition":"To lower into place and fix solidly, as the blocks of cut stone in a structure.","synonyms":[],"antonyms":[]},{"definition":"To wager in gambling; to risk.","synonyms":[],"antonyms":[]},{"definition":"To adorn with something infixed or affixed; to stud; to variegate with objects placed here and there.","synonyms":[],"antonyms":[]},{"definition":"To value; to rate; used with at.","synonyms":[],"antonyms":[]},{"definition":"To establish as a rule; to furnish; to prescribe; to assign.","synonyms":[],"antonyms":[],"example":"to set a good example"},{"definition":"To suit; to become.","synonyms":[],"antonyms":[],"example":"It sets him ill."}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lay,put,set down,light</x:t>
-  </x:si>
-  <x:si>
-    <x:t>extinguish,put out,quench,pick up</x:t>
-  </x:si>
-  <x:si>
-    <x:t>apple</x:t>
+    <x:t>words</x:t>
   </x:si>
   <x:si>
     <x:t>noun</x:t>
   </x:si>
   <x:si>
-    <x:t>/ˈæp.əl/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"definition":"A common, round fruit produced by the tree Malus domestica, cultivated in temperate climates.","synonyms":[],"antonyms":[]},{"definition":"Any of various tree-borne fruits or vegetables especially considered as resembling an apple; also (with qualifying words) used to form the names of other specific fruits such as custard apple, rose apple, thorn apple etc.","synonyms":[],"antonyms":[]},{"definition":"The fruit of the Tree of Knowledge, eaten by Adam and Eve according to post-Biblical Christian tradition; the forbidden fruit.","synonyms":[],"antonyms":[]},{"definition":"A tree of the genus Malus, especially one cultivated for its edible fruit; the apple tree.","synonyms":[],"antonyms":[]},{"definition":"The wood of the apple tree.","synonyms":[],"antonyms":[]},{"definition":"(in the plural) Short for apples and pears, slang for stairs.","synonyms":[],"antonyms":[]},{"definition":"The ball in baseball.","synonyms":[],"antonyms":[]},{"definition":"When smiling, the round, fleshy part of the cheeks between the eyes and the corners of the mouth.","synonyms":[],"antonyms":[]},{"definition":"A Native American or red-skinned person who acts and/or thinks like a white (Caucasian) person.","synonyms":[],"antonyms":[]},{"definition":"(ice hockey slang) An assist.","synonyms":[],"antonyms":[]}</x:t>
+    <x:t>/wɜːdz/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{"definition":"The smallest unit of language that has a particular meaning and can be expressed by itself; the smallest discrete, meaningful unit of language. (contrast morpheme.)","synonyms":[],"antonyms":[]},{"definition":"Something like such a unit of language:","synonyms":[],"antonyms":[]},{"definition":"The fact or act of speaking, as opposed to taking action. .","synonyms":[],"antonyms":[]},{"definition":"Something that someone said; a comment, utterance; speech.","synonyms":[],"antonyms":[]},{"definition":"A watchword or rallying cry, a verbal signal (even when consisting of multiple words).","synonyms":[],"antonyms":[],"example":"mum's the word"},{"definition":"A proverb or motto.","synonyms":[],"antonyms":[]},{"definition":"News; tidings (used without an article).","synonyms":[],"antonyms":[],"example":"Have you had any word from John yet?"},{"definition":"An order; a request or instruction; an expression of will.","synonyms":[],"antonyms":[],"example":"Don't fire till I give the word"},{"definition":"A promise; an oath or guarantee.","synonyms":["promise"],"antonyms":[],"example":"I give you my word that I will be there on time."},{"definition":"A brief discussion or conversation.","synonyms":[],"antonyms":[],"example":"Can I have a word with you?"},{"definition":"(in the plural) See words.","synonyms":[],"antonyms":[],"example":"There had been words between him and the secretary about the outcome of the meeting."},{"definition":"(sometimes Word) Communication from God; the message of the Christian gospel; the Bible, Scripture.","synonyms":["Bible","word of God"],"antonyms":[],"example":"Her parents had lived in Botswana, spreading the word among the tribespeople."},{"definition":"(sometimes Word) Logos, Christ.","synonyms":["God","Logos"],"antonyms":[]}</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bible,word of God,God,Logos,promise,vocable</x:t>
   </x:si>
   <x:si>
     <x:t/>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t>banana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/bəˈnɑːnə/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{"definition":"An elongated curved tropical fruit that grows in bunches and has a creamy flesh and a smooth skin.","synonyms":[],"antonyms":[]},{"definition":"The tropical tree-like plant which bears clusters of bananas. The plant, usually of the genus Musa but sometimes also including plants from Ensete, has large, elongated leaves and is related to the plantain.","synonyms":[],"antonyms":[]},{"definition":"A yellow colour, like that of a banana's skin.","synonyms":[],"antonyms":[]},{"definition":"(mildly) A person of Asian descent, especially a Chinese American, who has assimilated into Western culture or married a Caucasian (from the \"yellow\" outside and \"white\" inside). Compare coconut or Oreo.","synonyms":[],"antonyms":[]},{"definition":"A banana equivalent dose.","synonyms":[],"antonyms":[]},{"definition":"A catamorphism (from the use of banana brackets in the notation).","synonyms":[],"antonyms":[]},{"definition":"The penis.","synonyms":[],"antonyms":[]},{"definition":"A banana kick.","synonyms":[],"antonyms":[]}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Twinkie,jook-sing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>egg</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -485,46 +452,6 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:6">
-      <x:c r="A3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6">
-      <x:c r="A4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>